<commit_message>
WE ARE 5 WEEKS IN GANG
</commit_message>
<xml_diff>
--- a/Dagskrá.xlsx
+++ b/Dagskrá.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/884c6fd4e9c2b4f2/Documents/f_haskoli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{86EAC20A-716C-40B4-9A3E-579C1F623241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B44F78D-A3DA-4697-939E-C2C7DABB0CB3}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{86EAC20A-716C-40B4-9A3E-579C1F623241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8267584B-63F1-418A-B967-EE08E4BE8A36}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1350,7 +1350,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1395,7 +1395,7 @@
       <c r="P1" s="76"/>
       <c r="Q1" s="77">
         <f>(COUNTIF(C3:C26, TRUE)+COUNTIF(E3:E26, TRUE)+COUNTIF(G3:G26, TRUE)+COUNTIF(J3:J26, TRUE))/COUNTA(C3:C26,E3:E26,G3:G26,J3:J26)</f>
-        <v>0.38571428571428573</v>
+        <v>0.45714285714285713</v>
       </c>
       <c r="R1" s="78"/>
     </row>
@@ -1721,14 +1721,14 @@
         <v>41</v>
       </c>
       <c r="G11" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="47" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="23"/>
       <c r="J11" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="33" t="s">
         <v>42</v>
@@ -1744,7 +1744,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
       <c r="G12" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="48" t="s">
         <v>43</v>
@@ -1767,13 +1767,13 @@
         <v>45</v>
       </c>
       <c r="C13" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>46</v>

</xml_diff>